<commit_message>
Tests for ADD (8 and 16), ADC, SUB, SBC, DEC 16.
</commit_message>
<xml_diff>
--- a/op_code_progress.xlsx
+++ b/op_code_progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\projects\RustyGB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E02F446-6785-458C-92A9-DE7F756EACC8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{764A9222-5172-4711-80A6-C49FF5516EF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="opcodes" sheetId="1" r:id="rId1"/>
     <sheet name="prefixed" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="41">
   <si>
     <t>0x</t>
   </si>
@@ -146,12 +146,18 @@
   </si>
   <si>
     <t>Implemented and needs integration tests</t>
+  </si>
+  <si>
+    <t>Progress</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#\ ???/???"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -226,7 +232,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -296,6 +302,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -304,23 +328,30 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="4" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="60% - Accent2" xfId="4" builtinId="36"/>
@@ -329,7 +360,7 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -370,42 +401,6 @@
       <fill>
         <patternFill>
           <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -685,20 +680,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T17"/>
+  <dimension ref="A1:U17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K19" sqref="K19"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="19" max="19" width="3.85546875" customWidth="1"/>
     <col min="20" max="20" width="39.42578125" customWidth="1"/>
+    <col min="21" max="21" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>21</v>
@@ -749,7 +747,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -763,7 +761,7 @@
         <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s">
         <v>20</v>
@@ -778,13 +776,13 @@
         <v>37</v>
       </c>
       <c r="K2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="L2" t="s">
         <v>37</v>
       </c>
       <c r="M2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="N2" t="s">
         <v>20</v>
@@ -795,12 +793,15 @@
       <c r="P2" t="s">
         <v>37</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="S2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="T2" s="3"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T2" s="14"/>
+      <c r="U2" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -808,7 +809,7 @@
         <v>37</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
@@ -816,8 +817,11 @@
       <c r="G3" t="s">
         <v>20</v>
       </c>
+      <c r="K3" t="s">
+        <v>20</v>
+      </c>
       <c r="M3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="N3" t="s">
         <v>20</v>
@@ -825,17 +829,21 @@
       <c r="O3" t="s">
         <v>20</v>
       </c>
-      <c r="S3" s="8"/>
-      <c r="T3" s="9" t="s">
+      <c r="S3" s="9"/>
+      <c r="T3" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U3" s="10">
+        <f>COUNTIFS($B2:$Q17,"")</f>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
         <v>20</v>
@@ -843,8 +851,11 @@
       <c r="G4" t="s">
         <v>20</v>
       </c>
+      <c r="K4" t="s">
+        <v>20</v>
+      </c>
       <c r="M4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="N4" t="s">
         <v>20</v>
@@ -852,22 +863,29 @@
       <c r="O4" t="s">
         <v>20</v>
       </c>
-      <c r="S4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="T4" s="5" t="s">
+      <c r="S4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="T4" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U4" s="10">
+        <f>COUNTIFS($B2:$Q17,"x")</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>20</v>
+      </c>
+      <c r="K5" t="s">
+        <v>20</v>
       </c>
       <c r="M5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="N5" t="s">
         <v>20</v>
@@ -875,14 +893,18 @@
       <c r="O5" t="s">
         <v>20</v>
       </c>
-      <c r="S5" s="10" t="s">
+      <c r="S5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="T5" s="11" t="s">
+      <c r="T5" s="7" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U5" s="10">
+        <f>COUNTIFS($B2:$Q17,"i")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -928,14 +950,18 @@
       <c r="Q6" t="s">
         <v>20</v>
       </c>
-      <c r="S6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="T6" s="7" t="s">
+      <c r="S6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="T6" s="11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U6" s="12">
+        <f>COUNTIFS($B2:$Q17,"o")</f>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -982,7 +1008,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1029,7 +1055,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1055,121 +1081,205 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F10" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G10" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I10" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J10" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K10" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="L10" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="M10" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="N10" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="O10" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="Q10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="L11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="M11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="N11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="O11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="Q11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" t="s">
+        <v>17</v>
+      </c>
+      <c r="L12" t="s">
+        <v>17</v>
+      </c>
+      <c r="M12" t="s">
+        <v>17</v>
+      </c>
+      <c r="N12" t="s">
+        <v>17</v>
+      </c>
+      <c r="O12" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" t="s">
+        <v>17</v>
+      </c>
+      <c r="L13" t="s">
+        <v>17</v>
+      </c>
+      <c r="M13" t="s">
+        <v>17</v>
+      </c>
+      <c r="N13" t="s">
+        <v>17</v>
+      </c>
+      <c r="O13" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Completed tests for {AND, XOR, OR, CP} A, r8
</commit_message>
<xml_diff>
--- a/op_code_progress.xlsx
+++ b/op_code_progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\projects\RustyGB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{764A9222-5172-4711-80A6-C49FF5516EF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3326D77-E908-4FD5-A612-F4E2319213BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -686,7 +686,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomRight" activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,7 +871,7 @@
       </c>
       <c r="U4" s="10">
         <f>COUNTIFS($B2:$Q17,"x")</f>
-        <v>28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
@@ -958,7 +958,7 @@
       </c>
       <c r="U6" s="12">
         <f>COUNTIFS($B2:$Q17,"o")</f>
-        <v>104</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -1180,46 +1180,46 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="L12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="M12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="N12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="O12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="Q12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -1227,46 +1227,46 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G13" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I13" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J13" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K13" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="L13" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="M13" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="N13" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="O13" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="Q13" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Impl most arithmetic and logical ops
</commit_message>
<xml_diff>
--- a/op_code_progress.xlsx
+++ b/op_code_progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\projects\RustyGB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3326D77-E908-4FD5-A612-F4E2319213BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B86116-92D2-42B1-B637-B11305D69DE5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="41">
   <si>
     <t>0x</t>
   </si>
@@ -686,7 +686,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M20" sqref="M20"/>
+      <selection pane="bottomRight" activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,6 +808,9 @@
       <c r="C3" t="s">
         <v>37</v>
       </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
       <c r="E3" t="s">
         <v>20</v>
       </c>
@@ -817,9 +820,15 @@
       <c r="G3" t="s">
         <v>20</v>
       </c>
+      <c r="H3" t="s">
+        <v>37</v>
+      </c>
       <c r="K3" t="s">
         <v>20</v>
       </c>
+      <c r="L3" t="s">
+        <v>37</v>
+      </c>
       <c r="M3" t="s">
         <v>20</v>
       </c>
@@ -828,6 +837,9 @@
       </c>
       <c r="O3" t="s">
         <v>20</v>
+      </c>
+      <c r="P3" t="s">
+        <v>37</v>
       </c>
       <c r="S3" s="9"/>
       <c r="T3" s="5" t="s">
@@ -835,13 +847,19 @@
       </c>
       <c r="U3" s="10">
         <f>COUNTIFS($B2:$Q17,"")</f>
-        <v>117</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
       <c r="E4" t="s">
         <v>20</v>
       </c>
@@ -851,9 +869,15 @@
       <c r="G4" t="s">
         <v>20</v>
       </c>
+      <c r="H4" t="s">
+        <v>37</v>
+      </c>
       <c r="K4" t="s">
         <v>20</v>
       </c>
+      <c r="L4" t="s">
+        <v>37</v>
+      </c>
       <c r="M4" t="s">
         <v>20</v>
       </c>
@@ -862,6 +886,9 @@
       </c>
       <c r="O4" t="s">
         <v>20</v>
+      </c>
+      <c r="P4" t="s">
+        <v>37</v>
       </c>
       <c r="S4" s="2" t="s">
         <v>17</v>
@@ -878,12 +905,30 @@
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
       <c r="E5" t="s">
         <v>20</v>
       </c>
+      <c r="F5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" t="s">
+        <v>37</v>
+      </c>
       <c r="K5" t="s">
         <v>20</v>
       </c>
+      <c r="L5" t="s">
+        <v>37</v>
+      </c>
       <c r="M5" t="s">
         <v>20</v>
       </c>
@@ -892,6 +937,9 @@
       </c>
       <c r="O5" t="s">
         <v>20</v>
+      </c>
+      <c r="P5" t="s">
+        <v>37</v>
       </c>
       <c r="S5" s="4" t="s">
         <v>37</v>
@@ -901,7 +949,7 @@
       </c>
       <c r="U5" s="10">
         <f>COUNTIFS($B2:$Q17,"i")</f>
-        <v>7</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -926,6 +974,9 @@
       <c r="G6" t="s">
         <v>20</v>
       </c>
+      <c r="H6" t="s">
+        <v>37</v>
+      </c>
       <c r="I6" t="s">
         <v>20</v>
       </c>
@@ -946,6 +997,9 @@
       </c>
       <c r="O6" t="s">
         <v>20</v>
+      </c>
+      <c r="P6" t="s">
+        <v>37</v>
       </c>
       <c r="Q6" t="s">
         <v>20</v>
@@ -983,6 +1037,9 @@
       <c r="G7" t="s">
         <v>20</v>
       </c>
+      <c r="H7" t="s">
+        <v>37</v>
+      </c>
       <c r="I7" t="s">
         <v>20</v>
       </c>
@@ -1003,6 +1060,9 @@
       </c>
       <c r="O7" t="s">
         <v>20</v>
+      </c>
+      <c r="P7" t="s">
+        <v>37</v>
       </c>
       <c r="Q7" t="s">
         <v>20</v>
@@ -1030,6 +1090,9 @@
       <c r="G8" t="s">
         <v>20</v>
       </c>
+      <c r="H8" t="s">
+        <v>37</v>
+      </c>
       <c r="I8" t="s">
         <v>20</v>
       </c>
@@ -1050,6 +1113,9 @@
       </c>
       <c r="O8" t="s">
         <v>20</v>
+      </c>
+      <c r="P8" t="s">
+        <v>37</v>
       </c>
       <c r="Q8" t="s">
         <v>20</v>
@@ -1059,6 +1125,27 @@
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9" t="s">
+        <v>37</v>
+      </c>
       <c r="J9" t="s">
         <v>20</v>
       </c>
@@ -1076,6 +1163,9 @@
       </c>
       <c r="O9" t="s">
         <v>20</v>
+      </c>
+      <c r="P9" t="s">
+        <v>37</v>
       </c>
       <c r="Q9" t="s">
         <v>20</v>
@@ -1103,6 +1193,9 @@
       <c r="G10" t="s">
         <v>20</v>
       </c>
+      <c r="H10" t="s">
+        <v>37</v>
+      </c>
       <c r="I10" t="s">
         <v>20</v>
       </c>
@@ -1123,6 +1216,9 @@
       </c>
       <c r="O10" t="s">
         <v>20</v>
+      </c>
+      <c r="P10" t="s">
+        <v>37</v>
       </c>
       <c r="Q10" t="s">
         <v>20</v>
@@ -1150,6 +1246,9 @@
       <c r="G11" t="s">
         <v>20</v>
       </c>
+      <c r="H11" t="s">
+        <v>37</v>
+      </c>
       <c r="I11" t="s">
         <v>20</v>
       </c>
@@ -1170,6 +1269,9 @@
       </c>
       <c r="O11" t="s">
         <v>20</v>
+      </c>
+      <c r="P11" t="s">
+        <v>37</v>
       </c>
       <c r="Q11" t="s">
         <v>20</v>
@@ -1197,6 +1299,9 @@
       <c r="G12" t="s">
         <v>20</v>
       </c>
+      <c r="H12" t="s">
+        <v>37</v>
+      </c>
       <c r="I12" t="s">
         <v>20</v>
       </c>
@@ -1217,6 +1322,9 @@
       </c>
       <c r="O12" t="s">
         <v>20</v>
+      </c>
+      <c r="P12" t="s">
+        <v>37</v>
       </c>
       <c r="Q12" t="s">
         <v>20</v>
@@ -1244,6 +1352,9 @@
       <c r="G13" t="s">
         <v>20</v>
       </c>
+      <c r="H13" t="s">
+        <v>37</v>
+      </c>
       <c r="I13" t="s">
         <v>20</v>
       </c>
@@ -1264,6 +1375,9 @@
       </c>
       <c r="O13" t="s">
         <v>20</v>
+      </c>
+      <c r="P13" t="s">
+        <v>37</v>
       </c>
       <c r="Q13" t="s">
         <v>20</v>
@@ -1273,20 +1387,44 @@
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="H14" t="s">
+        <v>37</v>
+      </c>
+      <c r="P14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="H15" t="s">
+        <v>37</v>
+      </c>
+      <c r="P15" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>37</v>
+      </c>
+      <c r="P16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="H17" t="s">
+        <v>37</v>
+      </c>
+      <c r="P17" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed more opcode unit tests
</commit_message>
<xml_diff>
--- a/op_code_progress.xlsx
+++ b/op_code_progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\projects\RustyGB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B86116-92D2-42B1-B637-B11305D69DE5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E69A817B-7A24-4B43-9FE2-DBE29E692CD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5595" yWindow="2130" windowWidth="14700" windowHeight="9465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="opcodes" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="43">
   <si>
     <t>0x</t>
   </si>
@@ -79,9 +79,6 @@
     <t>Legend</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>Tested</t>
   </si>
   <si>
@@ -145,10 +142,19 @@
     <t>Implemented and only needs unit tests</t>
   </si>
   <si>
-    <t>Implemented and needs integration tests</t>
-  </si>
-  <si>
     <t>Progress</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>Implemented and needs integration or mocking unit tests</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>PREFIX</t>
   </si>
 </sst>
 </file>
@@ -328,7 +334,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="3" applyBorder="1"/>
@@ -346,6 +352,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -686,65 +693,65 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N14" sqref="N14"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="19" max="19" width="3.85546875" customWidth="1"/>
-    <col min="20" max="20" width="39.42578125" customWidth="1"/>
+    <col min="20" max="20" width="53.28515625" customWidth="1"/>
     <col min="21" max="21" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -752,53 +759,53 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P2" t="s">
-        <v>37</v>
-      </c>
-      <c r="S2" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="T2" s="14"/>
+      <c r="T2" s="15"/>
       <c r="U2" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -806,48 +813,48 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S3" s="9"/>
       <c r="T3" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U3" s="10">
         <f>COUNTIFS($B2:$Q17,"")</f>
-        <v>71</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -855,50 +862,53 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P4" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>39</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="T4" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" t="s">
-        <v>37</v>
-      </c>
-      <c r="K4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L4" t="s">
-        <v>37</v>
-      </c>
-      <c r="M4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O4" t="s">
-        <v>20</v>
-      </c>
-      <c r="P4" t="s">
-        <v>37</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="T4" s="6" t="s">
-        <v>38</v>
-      </c>
       <c r="U4" s="10">
-        <f>COUNTIFS($B2:$Q17,"x")</f>
-        <v>0</v>
+        <f>COUNTIFS($B2:$Q17,"u")</f>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
@@ -906,50 +916,56 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="H5" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="I5" t="s">
+        <v>39</v>
       </c>
       <c r="K5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P5" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>39</v>
       </c>
       <c r="S5" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T5" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="U5" s="10">
         <f>COUNTIFS($B2:$Q17,"i")</f>
-        <v>53</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -957,62 +973,62 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="T6" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="U6" s="12">
         <f>COUNTIFS($B2:$Q17,"o")</f>
-        <v>132</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -1020,52 +1036,52 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -1073,52 +1089,52 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -1126,49 +1142,49 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -1176,52 +1192,52 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -1229,52 +1245,52 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
@@ -1282,52 +1298,52 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -1335,96 +1351,189 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" t="s">
+        <v>36</v>
+      </c>
       <c r="H14" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="M14" t="s">
+        <v>42</v>
       </c>
       <c r="P14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" t="s">
+        <v>36</v>
+      </c>
       <c r="H15" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="M15" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="O15" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="P15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" t="s">
+        <v>36</v>
+      </c>
       <c r="H16" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="J16" t="s">
+        <v>36</v>
+      </c>
+      <c r="L16" t="s">
+        <v>36</v>
+      </c>
+      <c r="M16" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="N16" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="O16" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="P16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17" t="s">
+        <v>36</v>
+      </c>
       <c r="H17" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="J17" t="s">
+        <v>36</v>
+      </c>
+      <c r="K17" t="s">
+        <v>36</v>
+      </c>
+      <c r="L17" t="s">
+        <v>36</v>
+      </c>
+      <c r="M17" t="s">
+        <v>39</v>
+      </c>
+      <c r="N17" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="O17" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="P17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1439,10 +1548,10 @@
       <formula>"o"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
-      <formula>"x"</formula>
+      <formula>"u"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
-      <formula>""</formula>
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="notEqual">
+      <formula>" "</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
tests: added more CPU
</commit_message>
<xml_diff>
--- a/op_code_progress.xlsx
+++ b/op_code_progress.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\projects\RustyGB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E69A817B-7A24-4B43-9FE2-DBE29E692CD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCE330D-5C63-4409-A53D-B7852F2B8398}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5595" yWindow="2130" windowWidth="14700" windowHeight="9465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3135" yWindow="3120" windowWidth="14700" windowHeight="9465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="opcodes" sheetId="1" r:id="rId1"/>
@@ -693,7 +693,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomRight" activeCell="H5" sqref="H2:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,7 +777,7 @@
         <v>19</v>
       </c>
       <c r="H2" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="J2" t="s">
         <v>36</v>
@@ -828,7 +828,7 @@
         <v>19</v>
       </c>
       <c r="H3" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="K3" t="s">
         <v>19</v>
@@ -877,7 +877,7 @@
         <v>19</v>
       </c>
       <c r="H4" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="K4" t="s">
         <v>19</v>
@@ -931,7 +931,7 @@
         <v>19</v>
       </c>
       <c r="H5" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="I5" t="s">
         <v>39</v>
@@ -965,7 +965,7 @@
       </c>
       <c r="U5" s="10">
         <f>COUNTIFS($B2:$Q17,"i")</f>
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -1028,7 +1028,7 @@
       </c>
       <c r="U6" s="12">
         <f>COUNTIFS($B2:$Q17,"o")</f>
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
test: get rid of unecessary ownership in unittests
</commit_message>
<xml_diff>
--- a/op_code_progress.xlsx
+++ b/op_code_progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\projects\RustyGB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCE330D-5C63-4409-A53D-B7852F2B8398}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9003D3-E9E7-4618-8276-8E7EE1BDA23C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3135" yWindow="3120" windowWidth="14700" windowHeight="9465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-8190" yWindow="5160" windowWidth="14700" windowHeight="9465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="opcodes" sheetId="1" r:id="rId1"/>
@@ -693,7 +693,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H5" sqref="H2:H5"/>
+      <selection pane="bottomRight" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,7 +908,7 @@
       </c>
       <c r="U4" s="10">
         <f>COUNTIFS($B2:$Q17,"u")</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
@@ -934,7 +934,7 @@
         <v>19</v>
       </c>
       <c r="I5" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="K5" t="s">
         <v>19</v>
@@ -1028,7 +1028,7 @@
       </c>
       <c r="U6" s="12">
         <f>COUNTIFS($B2:$Q17,"o")</f>
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
feat: more CPU OPs
</commit_message>
<xml_diff>
--- a/op_code_progress.xlsx
+++ b/op_code_progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\projects\RustyGB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03860BEE-0D52-4CE7-9528-E0EE084A7B48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF434AE2-8882-4503-8A16-16C8AAE05113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-43050" yWindow="6735" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="opcodes" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="43">
   <si>
     <t>0x</t>
   </si>
@@ -164,7 +164,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#\ ???/???"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,8 +208,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -235,6 +242,11 @@
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
       </patternFill>
     </fill>
   </fills>
@@ -327,14 +339,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="3" applyBorder="1"/>
@@ -359,15 +372,60 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="5"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="60% - Accent2" xfId="4" builtinId="36"/>
+    <cellStyle name="Accent1" xfId="5" builtinId="29"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -690,10 +748,10 @@
   <dimension ref="A1:U17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N18" sqref="N18"/>
+      <selection pane="bottomRight" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,6 +837,9 @@
       <c r="H2" t="s">
         <v>19</v>
       </c>
+      <c r="I2" t="s">
+        <v>39</v>
+      </c>
       <c r="J2" t="s">
         <v>36</v>
       </c>
@@ -854,7 +915,7 @@
       </c>
       <c r="U3" s="10">
         <f>COUNTIFS($B2:$Q17,"")</f>
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -908,7 +969,7 @@
       </c>
       <c r="U4" s="10">
         <f>COUNTIFS($B2:$Q17,"u")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
@@ -1412,7 +1473,7 @@
       <c r="H14" t="s">
         <v>36</v>
       </c>
-      <c r="M14" t="s">
+      <c r="M14" s="16" t="s">
         <v>42</v>
       </c>
       <c r="P14" t="s">
@@ -1541,17 +1602,17 @@
     <mergeCell ref="S2:T2"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:Q17">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"i"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"o"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"u"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="notEqual">
-      <formula>" "</formula>
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+      <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>